<commit_message>
Update alarm table with new carousel alarms
</commit_message>
<xml_diff>
--- a/Input/reduced_filtered_AI_hmi_alarms.xlsx
+++ b/Input/reduced_filtered_AI_hmi_alarms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefano.massoletti.REGROUP\Desktop\LAVORO\Leonardo\_Generiche\Tool Nastri Leonardo\Nastrini-e-Coriandoli\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B21BF30-6E98-4342-8C79-F0D6A58B0CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319094CD-1C2A-4B8D-8634-8BE6B0F38038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" tabRatio="1000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4074" uniqueCount="1704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4083" uniqueCount="1717">
   <si>
     <t>0.0</t>
   </si>
@@ -5165,6 +5165,45 @@
   </si>
   <si>
     <t>CAROUSEL #: Safety breaker open fault.</t>
+  </si>
+  <si>
+    <t>CAROUSEL #: Carousel motor 1 not inserted</t>
+  </si>
+  <si>
+    <t>CARROUSEL # : Moteur du carrousel 1 non inséré</t>
+  </si>
+  <si>
+    <t>CAROUSEL #: Carousel motor 2 not inserted</t>
+  </si>
+  <si>
+    <t>CARROUSEL # : Moteur du carrousel 2 non inséré</t>
+  </si>
+  <si>
+    <t>CAROUSEL #: Carousel motor 3 not inserted</t>
+  </si>
+  <si>
+    <t>CARROUSEL # : Moteur du carrousel 3 non inséré</t>
+  </si>
+  <si>
+    <t>ALL_MOT_INSERTED_1</t>
+  </si>
+  <si>
+    <t>ALL_MOT_INSERTED_2</t>
+  </si>
+  <si>
+    <t>ALL_MOT_INSERTED_3</t>
+  </si>
+  <si>
+    <t>CAROUSEL MOTOR 1 NOT INSERTED</t>
+  </si>
+  <si>
+    <t>CAROUSEL MOTOR 2 NOT INSERTED</t>
+  </si>
+  <si>
+    <t>CAROUSEL MOTOR 3 NOT INSERTED</t>
+  </si>
+  <si>
+    <t>SAFETY BREAKER 3 OFF</t>
   </si>
 </sst>
 </file>
@@ -5488,13 +5527,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal 13" xfId="3" xr:uid="{300B754C-1DDD-4291-A3F2-A1076D1FAA56}"/>
@@ -13717,12 +13756,12 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="30" t="s">
+      <c r="A84" s="32" t="s">
         <v>532</v>
       </c>
-      <c r="B84" s="30"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="30"/>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
@@ -23765,8 +23804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23800,7 +23839,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="31">
+      <c r="A2" s="30">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -23818,7 +23857,7 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="31">
+      <c r="A3" s="30">
         <v>0.1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -23836,7 +23875,7 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="31">
+      <c r="A4" s="30">
         <v>0.2</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -23854,7 +23893,7 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="31">
+      <c r="A5" s="30">
         <v>0.3</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -23872,7 +23911,7 @@
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="31">
+      <c r="A6" s="30">
         <v>0.4</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -23890,7 +23929,7 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="31">
+      <c r="A7" s="30">
         <v>0.5</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -23908,7 +23947,7 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="31">
+      <c r="A8" s="30">
         <v>0.6</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -23926,7 +23965,7 @@
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="31">
+      <c r="A9" s="30">
         <v>0.7</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -23944,7 +23983,7 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="31">
+      <c r="A10" s="30">
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -23962,7 +24001,7 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="31">
+      <c r="A11" s="30">
         <v>1.1000000000000001</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -23980,7 +24019,7 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="31">
+      <c r="A12" s="30">
         <v>1.2</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -23998,7 +24037,7 @@
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="31">
+      <c r="A13" s="30">
         <v>1.3</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -24016,7 +24055,7 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="31">
+      <c r="A14" s="30">
         <v>1.4</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -24034,7 +24073,7 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="31">
+      <c r="A15" s="30">
         <v>1.5</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -24050,7 +24089,7 @@
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="31">
+      <c r="A16" s="30">
         <v>1.6</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -24066,7 +24105,7 @@
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="31">
+      <c r="A17" s="30">
         <v>1.7</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -24082,7 +24121,7 @@
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="31">
+      <c r="A18" s="30">
         <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -24100,7 +24139,7 @@
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="31">
+      <c r="A19" s="30">
         <v>2.1</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -24118,7 +24157,7 @@
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="31">
+      <c r="A20" s="30">
         <v>2.2000000000000002</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -24136,7 +24175,7 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="31">
+      <c r="A21" s="30">
         <v>2.2999999999999998</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -24154,7 +24193,7 @@
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="31">
+      <c r="A22" s="30">
         <v>2.4</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -24172,7 +24211,7 @@
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="31">
+      <c r="A23" s="30">
         <v>2.5</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -24190,7 +24229,7 @@
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="31">
+      <c r="A24" s="30">
         <v>2.6</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -24208,7 +24247,7 @@
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="31">
+      <c r="A25" s="30">
         <v>2.7</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -24226,7 +24265,7 @@
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="31">
+      <c r="A26" s="30">
         <v>3</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -24244,7 +24283,7 @@
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="31">
+      <c r="A27" s="30">
         <v>3.1</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -24262,7 +24301,7 @@
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="31">
+      <c r="A28" s="30">
         <v>3.2</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -24280,7 +24319,7 @@
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="31">
+      <c r="A29" s="30">
         <v>3.3</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -24298,7 +24337,7 @@
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="31">
+      <c r="A30" s="30">
         <v>3.4</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -24316,7 +24355,7 @@
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="31">
+      <c r="A31" s="30">
         <v>3.5</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -24334,7 +24373,7 @@
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="31">
+      <c r="A32" s="30">
         <v>3.6</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -24352,7 +24391,7 @@
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="31">
+      <c r="A33" s="30">
         <v>3.7</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -24370,7 +24409,7 @@
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="31">
+      <c r="A34" s="30">
         <v>4</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -24388,7 +24427,7 @@
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="31">
+      <c r="A35" s="30">
         <v>4.0999999999999996</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -24406,7 +24445,7 @@
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="31">
+      <c r="A36" s="30">
         <v>4.2</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -24424,7 +24463,7 @@
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="31">
+      <c r="A37" s="30">
         <v>4.3</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -24442,7 +24481,7 @@
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="31">
+      <c r="A38" s="30">
         <v>4.4000000000000004</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -24460,7 +24499,7 @@
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="31">
+      <c r="A39" s="30">
         <v>4.5</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -24478,7 +24517,7 @@
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="31">
+      <c r="A40" s="30">
         <v>4.5999999999999996</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -24496,7 +24535,7 @@
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="31">
+      <c r="A41" s="30">
         <v>4.7</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -24514,7 +24553,7 @@
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="31">
+      <c r="A42" s="30">
         <v>5</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -24532,7 +24571,7 @@
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="31">
+      <c r="A43" s="30">
         <v>5.0999999999999996</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -24550,7 +24589,7 @@
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="31">
+      <c r="A44" s="30">
         <v>5.2</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -24568,7 +24607,7 @@
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="31">
+      <c r="A45" s="30">
         <v>5.3</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -24586,7 +24625,7 @@
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="31">
+      <c r="A46" s="30">
         <v>5.4</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -24604,7 +24643,7 @@
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="31">
+      <c r="A47" s="30">
         <v>5.5</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -24622,39 +24661,51 @@
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="31">
+      <c r="A48" s="30">
         <v>5.6</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>150</v>
+        <v>1710</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="D48" s="5" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>1704</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>1705</v>
+      </c>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="31">
+      <c r="A49" s="30">
         <v>5.7</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>151</v>
+        <v>1711</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>1714</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>1707</v>
+      </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="31">
+      <c r="A50" s="30">
         <v>6</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -24676,7 +24727,7 @@
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="31">
+      <c r="A51" s="30">
         <v>6.1</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -24698,7 +24749,7 @@
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="31">
+      <c r="A52" s="30">
         <v>6.2</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -24720,7 +24771,7 @@
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="31">
+      <c r="A53" s="30">
         <v>6.3</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -24742,7 +24793,7 @@
       <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="31">
+      <c r="A54" s="30">
         <v>6.4</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -24754,7 +24805,7 @@
       <c r="D54" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="E54" s="32" t="s">
+      <c r="E54" s="31" t="s">
         <v>1364</v>
       </c>
       <c r="F54" s="5" t="s">
@@ -24764,7 +24815,7 @@
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="31">
+      <c r="A55" s="30">
         <v>6.5</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -24786,7 +24837,7 @@
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="31">
+      <c r="A56" s="30">
         <v>6.6</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -24808,7 +24859,7 @@
       <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="31">
+      <c r="A57" s="30">
         <v>6.7</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -24830,7 +24881,7 @@
       <c r="H57" s="5"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="31">
+      <c r="A58" s="30">
         <v>7</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -24852,7 +24903,7 @@
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="31">
+      <c r="A59" s="30">
         <v>7.1</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -24874,7 +24925,7 @@
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="31">
+      <c r="A60" s="30">
         <v>7.2</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -24896,7 +24947,7 @@
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="31">
+      <c r="A61" s="30">
         <v>7.3</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -24918,7 +24969,7 @@
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="31">
+      <c r="A62" s="30">
         <v>7.4</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -24940,7 +24991,7 @@
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="31">
+      <c r="A63" s="30">
         <v>7.5</v>
       </c>
       <c r="B63" s="5" t="s">
@@ -24962,7 +25013,7 @@
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="31">
+      <c r="A64" s="30">
         <v>7.6</v>
       </c>
       <c r="B64" s="5" t="s">
@@ -24984,7 +25035,7 @@
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" s="31">
+      <c r="A65" s="30">
         <v>7.7</v>
       </c>
       <c r="B65" s="5" t="s">
@@ -25000,7 +25051,7 @@
       <c r="H65" s="5"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="31">
+      <c r="A66" s="30">
         <v>8</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -25016,7 +25067,7 @@
       <c r="H66" s="5"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="31">
+      <c r="A67" s="30">
         <v>8.1</v>
       </c>
       <c r="B67" s="5" t="s">
@@ -25034,7 +25085,7 @@
       <c r="H67" s="5"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="31">
+      <c r="A68" s="30">
         <v>8.1999999999999993</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -25052,7 +25103,7 @@
       <c r="H68" s="5"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="31">
+      <c r="A69" s="30">
         <v>8.3000000000000007</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -25070,7 +25121,7 @@
       <c r="H69" s="5"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="31">
+      <c r="A70" s="30">
         <v>8.4</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -25086,7 +25137,7 @@
       <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71" s="31">
+      <c r="A71" s="30">
         <v>8.5</v>
       </c>
       <c r="B71" s="5" t="s">
@@ -25104,7 +25155,7 @@
       <c r="H71" s="5"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A72" s="31">
+      <c r="A72" s="30">
         <v>8.6</v>
       </c>
       <c r="B72" s="5" t="s">
@@ -25122,23 +25173,29 @@
       <c r="H72" s="5"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="31">
+      <c r="A73" s="30">
         <v>8.6999999999999993</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>175</v>
+        <v>1712</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
+      <c r="D73" s="5" t="s">
+        <v>1715</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>1708</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>1709</v>
+      </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="31">
+      <c r="A74" s="30">
         <v>9</v>
       </c>
       <c r="B74" s="5" t="s">
@@ -25160,7 +25217,7 @@
       <c r="H74" s="5"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="31">
+      <c r="A75" s="30">
         <v>9.1</v>
       </c>
       <c r="B75" s="5" t="s">
@@ -25170,7 +25227,7 @@
         <v>2</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>1142</v>
+        <v>1716</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -25178,7 +25235,7 @@
       <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A76" s="31">
+      <c r="A76" s="30">
         <v>9.1999999999999993</v>
       </c>
       <c r="B76" s="5" t="s">
@@ -25200,7 +25257,7 @@
       <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A77" s="31">
+      <c r="A77" s="30">
         <v>9.3000000000000007</v>
       </c>
       <c r="B77" s="5" t="s">
@@ -25222,7 +25279,7 @@
       <c r="H77" s="5"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A78" s="31">
+      <c r="A78" s="30">
         <v>9.4</v>
       </c>
       <c r="B78" s="5" t="s">
@@ -25244,7 +25301,7 @@
       <c r="H78" s="5"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A79" s="31">
+      <c r="A79" s="30">
         <v>9.5</v>
       </c>
       <c r="B79" s="5" t="s">
@@ -25266,7 +25323,7 @@
       <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A80" s="31">
+      <c r="A80" s="30">
         <v>9.6</v>
       </c>
       <c r="B80" s="5" t="s">
@@ -25288,7 +25345,7 @@
       <c r="H80" s="5"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A81" s="31">
+      <c r="A81" s="30">
         <v>9.6999999999999993</v>
       </c>
       <c r="B81" s="5" t="s">
@@ -25310,7 +25367,7 @@
       <c r="H81" s="5"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A82" s="31">
+      <c r="A82" s="30">
         <v>10</v>
       </c>
       <c r="B82" s="5" t="s">
@@ -25328,7 +25385,7 @@
       <c r="H82" s="5"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A83" s="31">
+      <c r="A83" s="30">
         <v>12</v>
       </c>
       <c r="B83" s="5" t="s">
@@ -25346,7 +25403,7 @@
       <c r="H83" s="5"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A84" s="31">
+      <c r="A84" s="30">
         <v>16</v>
       </c>
       <c r="B84" s="5" t="s">
@@ -25364,7 +25421,7 @@
       <c r="H84" s="5"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A85" s="31">
+      <c r="A85" s="30">
         <v>20</v>
       </c>
       <c r="B85" s="5" t="s">
@@ -25382,7 +25439,7 @@
       <c r="H85" s="5"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A86" s="31">
+      <c r="A86" s="30">
         <v>24</v>
       </c>
       <c r="B86" s="5" t="s">
@@ -25400,7 +25457,7 @@
       <c r="H86" s="5"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="31">
+      <c r="A87" s="30">
         <v>28</v>
       </c>
       <c r="B87" s="5" t="s">
@@ -25418,7 +25475,7 @@
       <c r="H87" s="5"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="31">
+      <c r="A88" s="30">
         <v>32</v>
       </c>
       <c r="B88" s="5" t="s">
@@ -25436,7 +25493,7 @@
       <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A89" s="31">
+      <c r="A89" s="30">
         <v>36</v>
       </c>
       <c r="B89" s="5" t="s">
@@ -25454,7 +25511,7 @@
       <c r="H89" s="5"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="31">
+      <c r="A90" s="30">
         <v>40</v>
       </c>
       <c r="B90" s="5" t="s">
@@ -25472,7 +25529,7 @@
       <c r="H90" s="5"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="31">
+      <c r="A91" s="30">
         <v>44</v>
       </c>
       <c r="B91" s="5" t="s">
@@ -25520,6 +25577,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010010850144F0DC324986F9A783986EC17C" ma:contentTypeVersion="15" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="46229f97138f5b47edc4079bd42a726f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xmlns:ns3="aca03388-b78c-4415-a826-d0bf4eb594c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae1af52ebfdbb73e4aed745e1e9600f5" ns2:_="" ns3:_="">
     <xsd:import namespace="383b0bb7-e620-4e20-ae9e-4f262a20ab07"/>
@@ -25738,15 +25804,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFE84900-1D66-40E2-A12A-E3BDA8DBE198}">
   <ds:schemaRefs>
@@ -25759,6 +25816,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617A2C0A-5DB5-4DBE-AFE9-CF838D0B604D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F42FBFE-7A75-46D3-8582-FF1095977D3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25775,12 +25840,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617A2C0A-5DB5-4DBE-AFE9-CF838D0B604D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Refactor file generation logic to include fixed zone handling and improve IO_LIST file retrieval. Updated `process_excel` and `generate_gen_line_file` functions to filter out zero trunk items and added a new utility function `find_io_list_file` for better file management. Enhanced GUI to support fixed emergency zone selection and improved logging capabilities.
</commit_message>
<xml_diff>
--- a/Input/reduced_filtered_AI_hmi_alarms.xlsx
+++ b/Input/reduced_filtered_AI_hmi_alarms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefano.massoletti.REGROUP\Desktop\LAVORO\Leonardo\_Generiche\Tool Nastri Leonardo\Nastrini-e-Coriandoli\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0C8C46-50E0-4CAC-98B6-4FBE44A136E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E1CECF-E52A-4900-B2F9-AEA752B0F5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" tabRatio="1000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SV DB" sheetId="18" r:id="rId1"/>
@@ -3733,9 +3733,6 @@
     <t>FIRESHUTTER #: FIRE ALARM detected.</t>
   </si>
   <si>
-    <t>SV_DV10001H</t>
-  </si>
-  <si>
     <t xml:space="preserve">CONVEYOR #: Alarms disabled by operator. </t>
   </si>
   <si>
@@ -5204,6 +5201,9 @@
   </si>
   <si>
     <t>CAROUSEL  : Moteur 3 - Défaut d'ouverture de l'interrupteur de sécurité.</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -5841,10 +5841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5852,9 +5852,10 @@
     <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>235</v>
       </c>
@@ -5862,10 +5863,13 @@
         <v>236</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1362</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>1204</v>
       </c>
@@ -5875,8 +5879,11 @@
       <c r="C2" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>1205</v>
       </c>
@@ -5886,8 +5893,11 @@
       <c r="C3" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>1206</v>
       </c>
@@ -5895,23 +5905,29 @@
         <v>304</v>
       </c>
       <c r="C4" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B5" s="8">
         <v>308</v>
       </c>
       <c r="C5" s="8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="D5" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="B6" s="8">
         <v>2306</v>
@@ -5919,8 +5935,11 @@
       <c r="C6" s="8">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>1207</v>
       </c>
@@ -5930,8 +5949,11 @@
       <c r="C7" s="8">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>1208</v>
       </c>
@@ -5941,8 +5963,11 @@
       <c r="C8" s="8">
         <v>120</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>1209</v>
       </c>
@@ -5950,10 +5975,13 @@
         <v>332</v>
       </c>
       <c r="C9" s="8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+      <c r="D9" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>1210</v>
       </c>
@@ -5961,10 +5989,13 @@
         <v>325</v>
       </c>
       <c r="C10" s="8">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>1211</v>
       </c>
@@ -5972,10 +6003,13 @@
         <v>342</v>
       </c>
       <c r="C11" s="8">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>440</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>1212</v>
       </c>
@@ -5983,10 +6017,13 @@
         <v>350</v>
       </c>
       <c r="C12" s="8">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+      <c r="D12" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>1213</v>
       </c>
@@ -5994,10 +6031,13 @@
         <v>376</v>
       </c>
       <c r="C13" s="8">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>1214</v>
       </c>
@@ -6005,10 +6045,13 @@
         <v>386</v>
       </c>
       <c r="C14" s="8">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>560</v>
+      </c>
+      <c r="D14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>1215</v>
       </c>
@@ -6016,10 +6059,13 @@
         <v>388</v>
       </c>
       <c r="C15" s="8">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>580</v>
+      </c>
+      <c r="D15" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>1216</v>
       </c>
@@ -6027,51 +6073,52 @@
         <v>322</v>
       </c>
       <c r="C16" s="8">
+        <v>610</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B17" s="8">
+        <v>326</v>
+      </c>
+      <c r="C17" s="8">
+        <v>620</v>
+      </c>
+      <c r="D17" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B18" s="8">
+        <v>306</v>
+      </c>
+      <c r="C18" s="8">
+        <v>630</v>
+      </c>
+      <c r="D18" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B19" s="9">
         <v>310</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>1226</v>
-      </c>
-      <c r="B17" s="8">
-        <v>398</v>
-      </c>
-      <c r="C17" s="8">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>1217</v>
-      </c>
-      <c r="B18" s="8">
-        <v>326</v>
-      </c>
-      <c r="C18" s="8">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>1218</v>
-      </c>
-      <c r="B19" s="8">
-        <v>306</v>
-      </c>
-      <c r="C19" s="8">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>1510</v>
-      </c>
-      <c r="B20" s="9">
-        <v>310</v>
-      </c>
-      <c r="C20" s="9">
-        <v>370</v>
+      <c r="C19" s="9">
+        <v>660</v>
+      </c>
+      <c r="D19" s="9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6115,10 +6162,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -6178,10 +6225,10 @@
         <v>715</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="F5" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -6198,10 +6245,10 @@
         <v>716</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="F6" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -6218,10 +6265,10 @@
         <v>717</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="F7" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -8001,10 +8048,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -8598,10 +8645,10 @@
         <v>756</v>
       </c>
       <c r="E41" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -8618,10 +8665,10 @@
         <v>757</v>
       </c>
       <c r="E42" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -8744,10 +8791,10 @@
         <v>759</v>
       </c>
       <c r="E51" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -8764,10 +8811,10 @@
         <v>760</v>
       </c>
       <c r="E52" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -8784,10 +8831,10 @@
         <v>761</v>
       </c>
       <c r="E53" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -8804,10 +8851,10 @@
         <v>762</v>
       </c>
       <c r="E54" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -8824,10 +8871,10 @@
         <v>763</v>
       </c>
       <c r="E55" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -8842,10 +8889,10 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -8862,10 +8909,10 @@
         <v>1038</v>
       </c>
       <c r="E57" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -8882,10 +8929,10 @@
         <v>1039</v>
       </c>
       <c r="E58" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -8902,10 +8949,10 @@
         <v>764</v>
       </c>
       <c r="E59" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -8922,10 +8969,10 @@
         <v>765</v>
       </c>
       <c r="E60" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -8942,10 +8989,10 @@
         <v>766</v>
       </c>
       <c r="E61" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -8962,10 +9009,10 @@
         <v>767</v>
       </c>
       <c r="E62" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -8982,10 +9029,10 @@
         <v>768</v>
       </c>
       <c r="E63" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -9000,10 +9047,10 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -9018,10 +9065,10 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -9036,10 +9083,10 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -9054,10 +9101,10 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -9072,10 +9119,10 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -9090,10 +9137,10 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -9108,10 +9155,10 @@
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -9220,7 +9267,7 @@
         <v>1219</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -9238,7 +9285,7 @@
         <v>1220</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -9282,7 +9329,7 @@
         <v>1221</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -9313,7 +9360,7 @@
         <v>1222</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -9357,7 +9404,7 @@
         <v>1224</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -10255,10 +10302,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -11051,10 +11098,10 @@
         <v>277</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="F58" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -11071,10 +11118,10 @@
         <v>278</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="F59" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -11091,10 +11138,10 @@
         <v>279</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="F60" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -11111,10 +11158,10 @@
         <v>280</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="F61" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -11131,10 +11178,10 @@
         <v>281</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F62" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -11151,10 +11198,10 @@
         <v>247</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="F63" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -11171,10 +11218,10 @@
         <v>285</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F64" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -11491,10 +11538,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
       <c r="G1" s="6"/>
     </row>
@@ -11655,10 +11702,10 @@
         <v>778</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="G11" s="6"/>
     </row>
@@ -11676,10 +11723,10 @@
         <v>780</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="G12" s="6"/>
     </row>
@@ -11697,10 +11744,10 @@
         <v>782</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="G13" s="6"/>
     </row>
@@ -11718,10 +11765,10 @@
         <v>784</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="G14" s="6"/>
     </row>
@@ -11933,10 +11980,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -12021,10 +12068,10 @@
         <v>800</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F6" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -12043,10 +12090,10 @@
         <v>802</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="F7" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -12065,10 +12112,10 @@
         <v>804</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="F8" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -12087,10 +12134,10 @@
         <v>806</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="F9" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -12109,10 +12156,10 @@
         <v>808</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F10" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -12131,10 +12178,10 @@
         <v>810</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="F11" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -12225,10 +12272,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -12303,10 +12350,10 @@
         <v>818</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F6" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -12491,10 +12538,10 @@
         <v>825</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="F19" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -12511,10 +12558,10 @@
         <v>826</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="F20" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -12531,10 +12578,10 @@
         <v>827</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="F21" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -12551,10 +12598,10 @@
         <v>828</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="F22" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -12571,10 +12618,10 @@
         <v>829</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="F23" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -12589,10 +12636,10 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="6" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="F24" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -12680,10 +12727,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -12863,10 +12910,10 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="6" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="F13" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -13189,10 +13236,10 @@
         <v>1191</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="F37" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -13209,10 +13256,10 @@
         <v>1025</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="F38" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -13229,10 +13276,10 @@
         <v>1181</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="F39" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -13249,10 +13296,10 @@
         <v>1182</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="F40" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -13269,10 +13316,10 @@
         <v>1183</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="F41" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -13289,10 +13336,10 @@
         <v>1184</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="F42" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -13309,10 +13356,10 @@
         <v>1185</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="F43" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -13329,10 +13376,10 @@
         <v>1186</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="F44" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -13349,10 +13396,10 @@
         <v>1187</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="F45" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -13369,10 +13416,10 @@
         <v>1188</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="F46" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -13389,10 +13436,10 @@
         <v>1189</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="F47" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -13409,10 +13456,10 @@
         <v>1190</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="F48" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -13429,10 +13476,10 @@
         <v>1026</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="F49" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -13449,10 +13496,10 @@
         <v>1027</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="F50" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -13469,10 +13516,10 @@
         <v>1176</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="F51" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -13489,10 +13536,10 @@
         <v>1177</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="F52" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -13509,10 +13556,10 @@
         <v>1180</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="F53" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -13529,10 +13576,10 @@
         <v>1028</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="F54" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -13549,10 +13596,10 @@
         <v>1029</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="F55" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -13569,10 +13616,10 @@
         <v>1030</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="F56" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -13589,10 +13636,10 @@
         <v>1031</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F57" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -13609,10 +13656,10 @@
         <v>1032</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="F58" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -13629,10 +13676,10 @@
         <v>1033</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="F59" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -13649,10 +13696,10 @@
         <v>1034</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="F60" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -13669,10 +13716,10 @@
         <v>1035</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="F61" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -13689,10 +13736,10 @@
         <v>1036</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="F62" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -13709,10 +13756,10 @@
         <v>1037</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="F63" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -13729,10 +13776,10 @@
         <v>1178</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="F64" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -13749,10 +13796,10 @@
         <v>1179</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="F65" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -13927,10 +13974,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -14256,10 +14303,10 @@
         <v>254</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="F23" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -14658,10 +14705,10 @@
         <v>272</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="F50" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -14678,10 +14725,10 @@
         <v>273</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="F51" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -14698,10 +14745,10 @@
         <v>274</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="F52" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -14718,10 +14765,10 @@
         <v>275</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="F53" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -14738,10 +14785,10 @@
         <v>276</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="F54" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -14758,10 +14805,10 @@
         <v>247</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="F55" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -14778,10 +14825,10 @@
         <v>874</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="F56" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -14826,10 +14873,10 @@
         <v>278</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="F59" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -14846,10 +14893,10 @@
         <v>279</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="F60" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -14866,10 +14913,10 @@
         <v>280</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="F61" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -14886,10 +14933,10 @@
         <v>281</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="F62" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -15225,10 +15272,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -15470,7 +15517,7 @@
         <v>1225</v>
       </c>
       <c r="F18" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -15487,10 +15534,10 @@
         <v>1171</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="F19" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -15719,10 +15766,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -15854,10 +15901,10 @@
         <v>1098</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="F10" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -15874,10 +15921,10 @@
         <v>1099</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="F11" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -15894,10 +15941,10 @@
         <v>1100</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="F12" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -16189,10 +16236,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -16222,10 +16269,10 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="6" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="F3" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -16430,10 +16477,10 @@
         <v>526</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="F18" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -16450,10 +16497,10 @@
         <v>527</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="F19" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -16470,10 +16517,10 @@
         <v>680</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="F20" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -16490,10 +16537,10 @@
         <v>528</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="F21" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -16510,10 +16557,10 @@
         <v>529</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="F22" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -16530,10 +16577,10 @@
         <v>530</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="F23" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -16550,10 +16597,10 @@
         <v>531</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="F24" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -18653,10 +18700,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -18703,10 +18750,10 @@
         <v>1163</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="F4" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -18923,10 +18970,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -18934,19 +18981,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="F2" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -18954,19 +19001,19 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="F3" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -18974,19 +19021,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="F4" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -18994,7 +19041,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
@@ -19007,7 +19054,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
@@ -19020,7 +19067,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>2</v>
@@ -19033,7 +19080,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2</v>
@@ -19046,7 +19093,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
@@ -19059,7 +19106,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -19072,7 +19119,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
@@ -19085,7 +19132,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
@@ -19170,7 +19217,7 @@
   </sheetPr>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B18" sqref="B18:E18"/>
     </sheetView>
   </sheetViews>
@@ -19199,10 +19246,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -19559,10 +19606,10 @@
         <v>696</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="F26" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -19579,10 +19626,10 @@
         <v>697</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="F27" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -19599,10 +19646,10 @@
         <v>698</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="F28" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -19619,10 +19666,10 @@
         <v>699</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="F29" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -20099,10 +20146,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -20239,10 +20286,10 @@
         <v>245</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="F10" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -20259,10 +20306,10 @@
         <v>246</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="F11" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -20279,10 +20326,10 @@
         <v>247</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="F12" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -20299,10 +20346,10 @@
         <v>248</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="F13" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -20637,10 +20684,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -20669,7 +20716,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -20879,10 +20926,10 @@
         <v>712</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="F18" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -20890,7 +20937,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>2</v>
@@ -20899,10 +20946,10 @@
         <v>270</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="F19" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -21106,7 +21153,7 @@
   </sheetPr>
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -21134,10 +21181,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -21145,7 +21192,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>2</v>
@@ -21156,7 +21203,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>2</v>
@@ -21167,7 +21214,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>2</v>
@@ -21178,7 +21225,7 @@
         <v>38</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>2</v>
@@ -21189,7 +21236,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>2</v>
@@ -21200,7 +21247,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>2</v>
@@ -21211,7 +21258,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>2</v>
@@ -21224,7 +21271,7 @@
         <v>102</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>2</v>
@@ -21237,7 +21284,7 @@
         <v>103</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>2</v>
@@ -21250,7 +21297,7 @@
         <v>104</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>2</v>
@@ -21263,7 +21310,7 @@
         <v>105</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>2</v>
@@ -21276,7 +21323,7 @@
         <v>106</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>2</v>
@@ -21289,7 +21336,7 @@
         <v>107</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="C14" s="29" t="s">
         <v>2</v>
@@ -21302,7 +21349,7 @@
         <v>108</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>2</v>
@@ -21315,7 +21362,7 @@
         <v>109</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="C16" s="29" t="s">
         <v>2</v>
@@ -21328,7 +21375,7 @@
         <v>110</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C17" s="29" t="s">
         <v>2</v>
@@ -21341,19 +21388,19 @@
         <v>111</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="29" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>1540</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>1541</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>1542</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -21361,19 +21408,19 @@
         <v>42</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="C19" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="29" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>1543</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>1544</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>1545</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -21381,19 +21428,19 @@
         <v>292</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="C20" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="29" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>1546</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>1547</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>1548</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -21401,19 +21448,19 @@
         <v>305</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C21" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="29" t="s">
+        <v>1548</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>1549</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>1550</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>1551</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -21421,19 +21468,19 @@
         <v>306</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="C22" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="29" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>1552</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>1553</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>1554</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -21441,19 +21488,19 @@
         <v>307</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="C23" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="29" t="s">
+        <v>1554</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>1555</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>1556</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>1557</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -21461,7 +21508,7 @@
         <v>308</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="C24" s="29" t="s">
         <v>2</v>
@@ -21475,7 +21522,7 @@
         <v>309</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="C25" s="29" t="s">
         <v>2</v>
@@ -21489,7 +21536,7 @@
         <v>310</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="C26" s="29" t="s">
         <v>2</v>
@@ -21503,7 +21550,7 @@
         <v>311</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="C27" s="29" t="s">
         <v>2</v>
@@ -21517,7 +21564,7 @@
         <v>465</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="C28" s="29" t="s">
         <v>2</v>
@@ -21531,7 +21578,7 @@
         <v>466</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="C29" s="29" t="s">
         <v>2</v>
@@ -21545,7 +21592,7 @@
         <v>467</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="C30" s="29" t="s">
         <v>2</v>
@@ -21559,7 +21606,7 @@
         <v>468</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="C31" s="29" t="s">
         <v>2</v>
@@ -21573,7 +21620,7 @@
         <v>469</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="C32" s="29" t="s">
         <v>2</v>
@@ -21587,7 +21634,7 @@
         <v>470</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="C33" s="29" t="s">
         <v>2</v>
@@ -21601,13 +21648,13 @@
         <v>471</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="C34" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -21617,13 +21664,13 @@
         <v>43</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="C35" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -21633,13 +21680,13 @@
         <v>472</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="C36" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -21649,13 +21696,13 @@
         <v>473</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -21665,13 +21712,13 @@
         <v>474</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="C38" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -21681,13 +21728,13 @@
         <v>475</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="C39" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -21697,13 +21744,13 @@
         <v>476</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="C40" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -21713,13 +21760,13 @@
         <v>477</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="C41" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -21729,13 +21776,13 @@
         <v>478</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="C42" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -21745,13 +21792,13 @@
         <v>479</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="C43" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -21761,13 +21808,13 @@
         <v>480</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="C44" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -21777,13 +21824,13 @@
         <v>481</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="C45" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -21793,13 +21840,13 @@
         <v>482</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C46" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -21809,13 +21856,13 @@
         <v>483</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="C47" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -21825,13 +21872,13 @@
         <v>484</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="C48" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -21841,13 +21888,13 @@
         <v>485</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C49" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -21857,13 +21904,13 @@
         <v>486</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="C50" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -21873,13 +21920,13 @@
         <v>44</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="C51" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -21889,13 +21936,13 @@
         <v>487</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C52" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -21905,13 +21952,13 @@
         <v>488</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C53" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -21921,13 +21968,13 @@
         <v>489</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="C54" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
@@ -21937,13 +21984,13 @@
         <v>490</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C55" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
@@ -21953,13 +22000,13 @@
         <v>491</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C56" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -21969,13 +22016,13 @@
         <v>492</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="C57" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -21985,141 +22032,141 @@
         <v>493</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C58" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C59" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="C60" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="27" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C61" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="27" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C62" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="27" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C63" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="27" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C64" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="C65" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D65" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="27" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="C66" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D66" s="29" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -22169,10 +22216,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -22279,10 +22326,10 @@
         <v>270</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F8" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -22447,10 +22494,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -22866,10 +22913,10 @@
         <v>259</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="F29" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -23049,10 +23096,10 @@
         <v>270</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="F41" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -23069,10 +23116,10 @@
         <v>271</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="F42" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -23180,10 +23227,10 @@
         <v>273</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="F50" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -23200,10 +23247,10 @@
         <v>272</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="F51" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -23220,10 +23267,10 @@
         <v>274</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="F52" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -23240,10 +23287,10 @@
         <v>275</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="F53" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -23260,10 +23307,10 @@
         <v>276</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="F54" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -23280,10 +23327,10 @@
         <v>247</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="F55" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -23298,10 +23345,10 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="6" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="F56" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -23316,10 +23363,10 @@
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="6" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="F57" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -23336,10 +23383,10 @@
         <v>277</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="F58" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -23356,10 +23403,10 @@
         <v>278</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="F59" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -23376,10 +23423,10 @@
         <v>279</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="F60" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -23396,10 +23443,10 @@
         <v>280</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="F61" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -23416,10 +23463,10 @@
         <v>281</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="F62" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -23434,10 +23481,10 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="6" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="F63" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -23452,10 +23499,10 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="6" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="F64" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -23567,10 +23614,10 @@
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="6" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="F72" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -23585,10 +23632,10 @@
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="6" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="F73" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -23629,10 +23676,10 @@
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="6" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="F76" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -23647,10 +23694,10 @@
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="6" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="F77" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -23665,10 +23712,10 @@
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="6" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="F78" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -23676,19 +23723,19 @@
         <v>17</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>1632</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="6" t="s">
         <v>1633</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="F79" t="s">
         <v>1634</v>
-      </c>
-      <c r="F79" t="s">
-        <v>1635</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -23804,7 +23851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E44" sqref="E44:F85"/>
     </sheetView>
   </sheetViews>
@@ -23832,10 +23879,10 @@
         <v>523</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>1364</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -24665,19 +24712,19 @@
         <v>5.6</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="E48" s="5" t="s">
+        <v>1666</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>1667</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>1668</v>
       </c>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
@@ -24687,19 +24734,19 @@
         <v>5.7</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="E49" s="5" t="s">
+        <v>1668</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>1669</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>1670</v>
       </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
@@ -24718,10 +24765,10 @@
         <v>273</v>
       </c>
       <c r="E50" s="5" t="s">
+        <v>1670</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>1671</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>1672</v>
       </c>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
@@ -24740,10 +24787,10 @@
         <v>274</v>
       </c>
       <c r="E51" s="5" t="s">
+        <v>1672</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>1673</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>1674</v>
       </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
@@ -24762,10 +24809,10 @@
         <v>274</v>
       </c>
       <c r="E52" s="5" t="s">
+        <v>1674</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>1675</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>1676</v>
       </c>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
@@ -24775,7 +24822,7 @@
         <v>6.3</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>2</v>
@@ -24784,10 +24831,10 @@
         <v>274</v>
       </c>
       <c r="E53" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>1677</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>1678</v>
       </c>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
@@ -24806,10 +24853,10 @@
         <v>275</v>
       </c>
       <c r="E54" s="31" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F54" s="5" t="s">
         <v>1679</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>1680</v>
       </c>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
@@ -24828,10 +24875,10 @@
         <v>276</v>
       </c>
       <c r="E55" s="5" t="s">
+        <v>1680</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>1681</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>1682</v>
       </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
@@ -24850,10 +24897,10 @@
         <v>247</v>
       </c>
       <c r="E56" s="5" t="s">
+        <v>1682</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>1683</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>1684</v>
       </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
@@ -24872,10 +24919,10 @@
         <v>1148</v>
       </c>
       <c r="E57" s="5" t="s">
+        <v>1684</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>1685</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>1686</v>
       </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
@@ -24894,10 +24941,10 @@
         <v>1149</v>
       </c>
       <c r="E58" s="5" t="s">
+        <v>1686</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>1687</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>1688</v>
       </c>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
@@ -24913,13 +24960,13 @@
         <v>2</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="E59" s="5" t="s">
+        <v>1688</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>1689</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>1690</v>
       </c>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
@@ -24935,13 +24982,13 @@
         <v>2</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="E60" s="5" t="s">
+        <v>1690</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>1691</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>1692</v>
       </c>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
@@ -24957,13 +25004,13 @@
         <v>2</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="E61" s="5" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>1693</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>1694</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
@@ -24979,13 +25026,13 @@
         <v>2</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="E62" s="5" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>1695</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>1696</v>
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
@@ -25001,13 +25048,13 @@
         <v>2</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="E63" s="5" t="s">
+        <v>1696</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>1697</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>1698</v>
       </c>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
@@ -25017,19 +25064,19 @@
         <v>7.6</v>
       </c>
       <c r="B64" s="5" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>1643</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>1644</v>
-      </c>
       <c r="E64" s="5" t="s">
+        <v>1698</v>
+      </c>
+      <c r="F64" s="5" t="s">
         <v>1699</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>1700</v>
       </c>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
@@ -25177,19 +25224,19 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="E73" s="5" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F73" s="5" t="s">
         <v>1701</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>1702</v>
       </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
@@ -25199,19 +25246,19 @@
         <v>9</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="E74" s="5" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F74" s="5" t="s">
         <v>1703</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>1704</v>
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
@@ -25221,13 +25268,13 @@
         <v>9.1</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -25239,19 +25286,19 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="E76" s="5" t="s">
+        <v>1704</v>
+      </c>
+      <c r="F76" s="5" t="s">
         <v>1705</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>1706</v>
       </c>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
@@ -25261,19 +25308,19 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E77" s="5" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F77" s="5" t="s">
         <v>1707</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>1708</v>
       </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
@@ -25283,19 +25330,19 @@
         <v>9.4</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="E78" s="5" t="s">
+        <v>1708</v>
+      </c>
+      <c r="F78" s="5" t="s">
         <v>1709</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>1710</v>
       </c>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
@@ -25305,7 +25352,7 @@
         <v>9.5</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>2</v>
@@ -25314,10 +25361,10 @@
         <v>272</v>
       </c>
       <c r="E79" s="5" t="s">
+        <v>1710</v>
+      </c>
+      <c r="F79" s="5" t="s">
         <v>1711</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>1712</v>
       </c>
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
@@ -25327,7 +25374,7 @@
         <v>9.6</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>2</v>
@@ -25336,10 +25383,10 @@
         <v>272</v>
       </c>
       <c r="E80" s="5" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F80" s="5" t="s">
         <v>1713</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>1714</v>
       </c>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
@@ -25349,7 +25396,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>2</v>
@@ -25358,10 +25405,10 @@
         <v>272</v>
       </c>
       <c r="E81" s="5" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F81" s="5" t="s">
         <v>1715</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>1716</v>
       </c>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
@@ -25425,13 +25472,13 @@
         <v>20</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>187</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
@@ -25497,13 +25544,13 @@
         <v>36</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>189</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
@@ -25515,13 +25562,13 @@
         <v>40</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>187</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
@@ -25533,13 +25580,13 @@
         <v>44</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>189</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
@@ -25781,15 +25828,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <MigrationWizIdPermissions xmlns="383b0bb7-e620-4e20-ae9e-4f262a20ab07" xsi:nil="true"/>
@@ -25802,6 +25840,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25824,14 +25871,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617A2C0A-5DB5-4DBE-AFE9-CF838D0B604D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFE84900-1D66-40E2-A12A-E3BDA8DBE198}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -25840,4 +25879,12 @@
     <ds:schemaRef ds:uri="aca03388-b78c-4415-a826-d0bf4eb594c5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617A2C0A-5DB5-4DBE-AFE9-CF838D0B604D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>